<commit_message>
full file restructure, and report finished (i think)
</commit_message>
<xml_diff>
--- a/dataGen/empiricalData.xlsx
+++ b/dataGen/empiricalData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="totalRuntimes" sheetId="1" state="visible" r:id="rId3"/>
@@ -3020,7 +3020,7 @@
   </sheetPr>
   <dimension ref="A1:W9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="P15" activeCellId="0" sqref="P15"/>
     </sheetView>
   </sheetViews>
@@ -4399,7 +4399,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4523,7 +4523,7 @@
         <v>1000</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>0.012</v>
+        <v>0.01</v>
       </c>
       <c r="E6" s="3" t="n">
         <v>0.26</v>
@@ -4563,7 +4563,7 @@
         <v>4000</v>
       </c>
       <c r="D8" s="3" t="n">
-        <v>0.046</v>
+        <v>0.05</v>
       </c>
       <c r="E8" s="3" t="n">
         <v>4.2</v>
@@ -4583,7 +4583,7 @@
         <v>8000</v>
       </c>
       <c r="D9" s="3" t="n">
-        <v>0.096</v>
+        <v>0.1</v>
       </c>
       <c r="E9" s="3" t="n">
         <v>16.6</v>
@@ -4610,8 +4610,8 @@
   </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>